<commit_message>
Modif VueMenu version mobile
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17895" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20985" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -33,9 +34,6 @@
     <t xml:space="preserve">      M'inscrire à la soirée des anciens</t>
   </si>
   <si>
-    <t xml:space="preserve">      Consulter la liste des inscrits</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Modifier mon inscription</t>
   </si>
   <si>
@@ -45,9 +43,6 @@
     <t>Le réseau des anciens élèves</t>
   </si>
   <si>
-    <t xml:space="preserve">      Rechercher d'autres anciens</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Proposer un stage à un étudiant</t>
   </si>
   <si>
@@ -57,18 +52,12 @@
     <t>Gestion du menu administrateur</t>
   </si>
   <si>
-    <t xml:space="preserve">      Modifier les informations sur la soirée</t>
-  </si>
-  <si>
     <t>La soirée annuelle des anciens</t>
   </si>
   <si>
     <t xml:space="preserve">      Envoyer un courriel de relance</t>
   </si>
   <si>
-    <t xml:space="preserve">      Mettre à jour les réglements et remboursements</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Gérer la galerie de photos</t>
   </si>
   <si>
@@ -118,6 +107,21 @@
   </si>
   <si>
     <t>Développement en PHP de l'application web de gestion des anciens élèves du BTS SIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Consulter les infos sur la soirée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Consulter la liste des inscriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Rechercher d'autres anciens élèves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Modifier les infos sur la soirée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Mettre à jour réglements et remboursements</t>
   </si>
 </sst>
 </file>
@@ -215,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -229,6 +233,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -534,10 +541,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -552,14 +559,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="6"/>
@@ -570,18 +577,18 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -592,19 +599,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75">
@@ -617,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -629,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -638,310 +645,352 @@
     </row>
     <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" customFormat="1">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" customFormat="1">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" customFormat="1">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" customFormat="1">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6">
+    <row r="17" spans="1:6" customFormat="1">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" customFormat="1">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" customFormat="1">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    <row r="22" spans="1:6" customFormat="1">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="25" spans="1:6" customFormat="1" ht="18.75">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
-      <c r="A26" s="1" t="s">
+      <c r="F25" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" customFormat="1">
+      <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75">
-      <c r="A30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6">
+    <row r="29" spans="1:6" customFormat="1">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="31" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" customFormat="1">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" customFormat="1">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" customFormat="1">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75">
-      <c r="A36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6">
+    <row r="35" spans="1:6" customFormat="1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="37" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" customFormat="1">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6">
+    <row r="39" spans="1:6" customFormat="1">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="41" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" customFormat="1">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" customFormat="1">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75">
-      <c r="A45" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6">
+    <row r="44" spans="1:6" customFormat="1">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="46" spans="1:6" customFormat="1" ht="15.75">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" customFormat="1">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" customFormat="1">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" customFormat="1">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Réorganisation des menus de la version mobile avec un système d'accordéon + renommage de nombreux fichiers
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20985" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -127,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +250,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -296,7 +304,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,9 +336,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,6 +371,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,17 +547,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
@@ -558,7 +568,7 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -568,7 +578,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -576,7 +586,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>28</v>
       </c>
@@ -586,7 +596,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
@@ -594,7 +604,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -614,12 +624,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -631,7 +641,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -643,12 +653,12 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" customFormat="1">
+    <row r="13" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -660,7 +670,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1">
+    <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -672,7 +682,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1">
+    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -684,7 +694,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" customFormat="1">
+    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -696,7 +706,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1">
+    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -708,7 +718,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="15.75">
+    <row r="19" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -718,7 +728,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1">
+    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -730,7 +740,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1">
+    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -742,7 +752,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1">
+    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -754,7 +764,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="18.75">
+    <row r="25" spans="1:6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -774,7 +784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -784,7 +794,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1">
+    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -796,7 +806,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" customFormat="1">
+    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -808,7 +818,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="31" spans="1:6" customFormat="1" ht="15.75">
+    <row r="31" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -818,7 +828,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1">
+    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -830,7 +840,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1">
+    <row r="33" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -842,7 +852,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1">
+    <row r="34" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -854,7 +864,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" customFormat="1">
+    <row r="35" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -866,7 +876,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="37" spans="1:6" customFormat="1" ht="15.75">
+    <row r="37" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -876,7 +886,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" customFormat="1">
+    <row r="38" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -888,7 +898,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" customFormat="1">
+    <row r="39" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -900,7 +910,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="41" spans="1:6" customFormat="1" ht="15.75">
+    <row r="41" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -910,7 +920,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" customFormat="1">
+    <row r="42" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -922,7 +932,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" customFormat="1">
+    <row r="43" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -934,7 +944,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" customFormat="1">
+    <row r="44" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -946,7 +956,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="46" spans="1:6" customFormat="1" ht="15.75">
+    <row r="46" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -956,7 +966,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" customFormat="1">
+    <row r="47" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -968,7 +978,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" customFormat="1">
+    <row r="48" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -980,7 +990,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" customFormat="1">
+    <row r="49" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1003,24 +1013,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Améliorations du changement de mdp et de la modification du profil perso
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="8070"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16230" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -127,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,6 +239,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -304,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,10 +339,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,7 +373,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,17 +548,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
@@ -568,17 +569,17 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -586,17 +587,17 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
@@ -604,7 +605,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -624,41 +625,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="9">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="9">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" customFormat="1">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -670,7 +675,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" customFormat="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -682,7 +687,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" customFormat="1">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -694,7 +699,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" customFormat="1">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -706,7 +711,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" customFormat="1">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -718,7 +723,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" customFormat="1" ht="15.75">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -728,7 +733,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" customFormat="1">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -740,7 +745,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" customFormat="1">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -752,7 +757,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" customFormat="1">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -764,7 +769,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" customFormat="1" ht="18.75">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -784,7 +789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" customFormat="1" ht="15.75">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -794,19 +799,21 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" customFormat="1">
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="9">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" customFormat="1">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -818,7 +825,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="31" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" customFormat="1" ht="15.75">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -828,7 +835,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" customFormat="1">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -840,7 +847,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" customFormat="1">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -852,7 +859,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" customFormat="1">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -864,7 +871,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" customFormat="1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -876,7 +883,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="37" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" customFormat="1" ht="15.75">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -886,7 +893,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" customFormat="1">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -898,7 +905,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" customFormat="1">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -910,7 +917,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="41" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" customFormat="1" ht="15.75">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -920,7 +927,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" customFormat="1">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -932,7 +939,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" customFormat="1">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -944,7 +951,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" customFormat="1">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -956,7 +963,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="46" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" customFormat="1" ht="15.75">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -966,7 +973,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" customFormat="1">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -978,7 +985,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" customFormat="1">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -990,7 +997,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" customFormat="1">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1013,24 +1020,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifications du profil Administrateur
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16230" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -127,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,9 +339,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,6 +374,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -548,17 +550,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
@@ -569,7 +571,7 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
@@ -579,7 +581,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -587,7 +589,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
@@ -597,7 +599,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
@@ -605,7 +607,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -625,12 +627,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -644,7 +646,7 @@
         <v>42512</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -658,12 +660,12 @@
         <v>42512</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" customFormat="1">
+    <row r="13" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -675,7 +677,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1">
+    <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -687,7 +689,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1">
+    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -699,7 +701,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" customFormat="1">
+    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -711,7 +713,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1">
+    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -723,7 +725,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="15.75">
+    <row r="19" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -733,7 +735,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1">
+    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -745,7 +747,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1">
+    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -757,7 +759,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1">
+    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -769,7 +771,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="18.75">
+    <row r="25" spans="1:6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -789,7 +791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -799,7 +801,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1">
+    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -813,19 +815,23 @@
         <v>42512</v>
       </c>
     </row>
-    <row r="29" spans="1:6" customFormat="1">
+    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="31" spans="1:6" customFormat="1" ht="15.75">
+      <c r="D29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="9">
+        <v>42514</v>
+      </c>
+      <c r="F29" s="9">
+        <v>42514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -835,19 +841,19 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1">
+    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1">
+    <row r="33" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -859,7 +865,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1">
+    <row r="34" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -871,7 +877,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" customFormat="1">
+    <row r="35" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -883,7 +889,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="37" spans="1:6" customFormat="1" ht="15.75">
+    <row r="37" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -893,7 +899,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" customFormat="1">
+    <row r="38" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -905,7 +911,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" customFormat="1">
+    <row r="39" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -917,7 +923,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="41" spans="1:6" customFormat="1" ht="15.75">
+    <row r="41" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -927,7 +933,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" customFormat="1">
+    <row r="42" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -939,7 +945,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" customFormat="1">
+    <row r="43" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -951,7 +957,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" customFormat="1">
+    <row r="44" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -963,7 +969,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="46" spans="1:6" customFormat="1" ht="15.75">
+    <row r="46" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -973,7 +979,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" customFormat="1">
+    <row r="47" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -985,7 +991,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" customFormat="1">
+    <row r="48" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -997,7 +1003,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" customFormat="1">
+    <row r="49" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1020,24 +1026,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification de la classe "Inscription.class.php", celle-ci ne convertit plus la date au format US puisqu'elle est déjà sous format US au submit (dans mon cas).
Faire un test si la date au "submit" est au format US => Ne rien faire,
ou au format FR => la convertir au format US
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -556,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,9 @@
         <v>26</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="E32" s="9">
+        <v>42514</v>
+      </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modifications des fautes d'orthographes. Modifications de la modification des infos de la soirée et des vues
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -556,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,9 +672,13 @@
       <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="9">
+        <v>42515</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Améliorations de la DAO, de la classe "Outils" des contrôleurs et des vues de "CreerCompteAdmin", "CreerCompteEleve", "CreerMonInscription", "VoirDetailsSoiree" + Création du contrôleur et des vues de "VoisListeInscrits"
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="6240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -556,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,9 +669,7 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
@@ -697,12 +695,14 @@
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="9">
+        <v>42515</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
@@ -863,12 +863,14 @@
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="9">
+        <v>42515</v>
+      </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Améliorations des vues "VoirListeInscrits" et autres vues + liste des tâches modifié et vérification de test des vues modifier élève/admin, supprimer élève/admin
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="6240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">      Mettre à jour réglements et remboursements</t>
+  </si>
+  <si>
+    <t>Mise en forme restante</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -242,6 +245,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -554,10 +560,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,49 +571,54 @@
     <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -618,94 +629,102 @@
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="9">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="9">
         <v>42512</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="9">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="9">
         <v>42512</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="9">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="9">
         <v>42515</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="9">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="9">
         <v>42515</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -716,8 +735,9 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -728,8 +748,9 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="19" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="19" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -738,8 +759,9 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -750,20 +772,22 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -774,8 +798,9 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="25" spans="1:6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="25" spans="1:7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -786,16 +811,19 @@
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -804,38 +832,41 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="9">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="9">
         <v>42512</v>
       </c>
     </row>
-    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="9">
-        <v>42514</v>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F29" s="9">
         <v>42514</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="9">
+        <v>42514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -844,36 +875,41 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="9">
+      <c r="E32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="9">
         <v>42514</v>
       </c>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="9">
+        <v>42516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="9">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="9">
         <v>42515</v>
       </c>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -884,8 +920,9 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -896,8 +933,9 @@
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-    </row>
-    <row r="37" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="37" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -906,8 +944,9 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -918,8 +957,9 @@
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -930,8 +970,9 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-    </row>
-    <row r="41" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+    </row>
+    <row r="41" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -940,20 +981,24 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="E42" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="9">
+        <v>42516</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -964,8 +1009,9 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -976,8 +1022,9 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-    </row>
-    <row r="46" spans="1:6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G44" s="5"/>
+    </row>
+    <row r="46" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1033,9 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -998,8 +1046,9 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -1010,8 +1059,9 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1022,11 +1072,12 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Améliorations et finitions des vues "VoirListeInscrits" pour la partie anciens élèves et administrateur. Modification de la classe DAO et son test, de la classe Inscription et son test, de la page index (ajout de VoirListeInscritsEleve et Admin) ainsi que les vues et contrôleurs "CreerMonInscription"
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -562,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,14 +715,16 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F15" s="9">
         <v>42515</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="9">
+        <v>42517</v>
+      </c>
     </row>
     <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -900,14 +902,16 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F33" s="9">
         <v>42515</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="9">
+        <v>42517</v>
+      </c>
     </row>
     <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -993,7 +997,9 @@
       <c r="E42" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="F42" s="9">
+        <v>42516</v>
+      </c>
       <c r="G42" s="9">
         <v>42516</v>
       </c>
@@ -1002,14 +1008,18 @@
       <c r="A43" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G43" s="9">
+        <v>42517</v>
+      </c>
     </row>
     <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1039,14 +1049,18 @@
       <c r="A47" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G47" s="9">
+        <v>42517</v>
+      </c>
     </row>
     <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1058,8 +1072,8 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">

</xml_diff>

<commit_message>
Modifications de vues + classe DAO + Modification du contrôleur et des vues pour modifier/supprimer une inscription avec envoie de mail en fonction de ce qu'il reste à être rembourser ou à payer + création d'un script de génération d'adresses mails
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -562,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +656,9 @@
       <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="9">
+        <v>42512</v>
+      </c>
       <c r="G9" s="9">
         <v>42512</v>
       </c>
@@ -671,7 +673,9 @@
       <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="9">
+        <v>42512</v>
+      </c>
       <c r="G10" s="9">
         <v>42512</v>
       </c>
@@ -694,7 +698,9 @@
       <c r="F13" s="9">
         <v>42515</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="9">
+        <v>42516</v>
+      </c>
     </row>
     <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -706,8 +712,12 @@
         <v>26</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="9">
+        <v>42516</v>
+      </c>
+      <c r="G14" s="9">
+        <v>42516</v>
+      </c>
     </row>
     <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -730,27 +740,35 @@
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G16" s="9">
+        <v>42520</v>
+      </c>
     </row>
     <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G17" s="9">
+        <v>42520</v>
+      </c>
     </row>
     <row r="19" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -786,8 +804,12 @@
         <v>26</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="F21" s="9">
+        <v>42514</v>
+      </c>
+      <c r="G21" s="9">
+        <v>42514</v>
+      </c>
     </row>
     <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -846,7 +868,9 @@
       <c r="E28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="9">
+        <v>42512</v>
+      </c>
       <c r="G28" s="9">
         <v>42512</v>
       </c>

</xml_diff>

<commit_message>
Amélioration et création du contrôleur et des vues ModifierReglementsRemboursements + de la vue jquery "Connecter" + les vues "Menu"
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -55,9 +55,6 @@
     <t>La soirée annuelle des anciens</t>
   </si>
   <si>
-    <t xml:space="preserve">      Envoyer un courriel de relance</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Gérer la galerie de photos</t>
   </si>
   <si>
@@ -125,6 +122,12 @@
   </si>
   <si>
     <t>Mise en forme restante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Envoyer un courriel</t>
+  </si>
+  <si>
+    <t>courriel : une personne, tout le monde, les inscrits, les non inscrits, une année de début de BTS</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +583,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -600,7 +603,7 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -623,22 +626,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -654,7 +657,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="9">
         <v>42512</v>
@@ -671,7 +674,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="9">
         <v>42512</v>
@@ -692,7 +695,7 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="9">
@@ -704,12 +707,12 @@
     </row>
     <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="9">
@@ -721,13 +724,13 @@
     </row>
     <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="9">
         <v>42515</v>
@@ -743,7 +746,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9">
@@ -760,7 +763,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9">
@@ -783,10 +786,10 @@
     </row>
     <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -801,7 +804,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="9">
@@ -816,7 +819,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -824,27 +827,32 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="25" spans="1:7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -866,7 +874,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" s="9">
         <v>42512</v>
@@ -883,7 +891,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="9">
         <v>42514</v>
@@ -905,13 +913,13 @@
     </row>
     <row r="32" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F32" s="9">
         <v>42514</v>
@@ -922,13 +930,13 @@
     </row>
     <row r="33" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33" s="9">
         <v>42515</v>
@@ -939,10 +947,10 @@
     </row>
     <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -952,10 +960,10 @@
     </row>
     <row r="35" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -976,10 +984,10 @@
     </row>
     <row r="38" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -989,10 +997,10 @@
     </row>
     <row r="39" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1002,7 +1010,7 @@
     </row>
     <row r="41" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1013,13 +1021,13 @@
     </row>
     <row r="42" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F42" s="9">
         <v>42516</v>
@@ -1030,13 +1038,13 @@
     </row>
     <row r="43" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F43" s="9">
         <v>42517</v>
@@ -1047,10 +1055,10 @@
     </row>
     <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1060,7 +1068,7 @@
     </row>
     <row r="46" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1071,13 +1079,13 @@
     </row>
     <row r="47" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F47" s="9">
         <v>42517</v>
@@ -1088,10 +1096,10 @@
     </row>
     <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1101,10 +1109,10 @@
     </row>
     <row r="49" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>

</xml_diff>

<commit_message>
Modification du contrôleur et des vues VoirDetailsSoiree + modification du fichier parametres.localhost pour le script d'export en CSV (fonctionne) + ajout image explication dans documents : "ouvrir csv en utf8 dans excel" + documentation envoi de mail (+ test envoie de mail fonctionnent en i12, mais limite de 120 secondes à régler (230 mails envoyés environ))
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>courriel : une personne, tout le monde, les inscrits, les non inscrits, une année de début de BTS</t>
+  </si>
+  <si>
+    <t>Adresse mailchimp : delasalle.sio.destinataire@gmail.com</t>
+  </si>
+  <si>
+    <t>mdp : Sio1_Sio2</t>
   </si>
 </sst>
 </file>
@@ -563,10 +569,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +762,7 @@
         <v>42520</v>
       </c>
     </row>
-    <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -773,7 +779,7 @@
         <v>42520</v>
       </c>
     </row>
-    <row r="19" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -784,7 +790,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -797,7 +803,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -814,7 +820,7 @@
         <v>42514</v>
       </c>
     </row>
-    <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -827,12 +833,18 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -855,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -866,7 +878,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -883,7 +895,7 @@
         <v>42512</v>
       </c>
     </row>
-    <row r="29" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -900,7 +912,7 @@
         <v>42514</v>
       </c>
     </row>
-    <row r="31" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -911,7 +923,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -962,14 +974,18 @@
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="9">
+        <v>42521</v>
+      </c>
+      <c r="G35" s="9">
+        <v>42522</v>
+      </c>
     </row>
     <row r="37" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">

</xml_diff>

<commit_message>
Création et début contrôleur et les vues "ExporterLesDonnées + essais d'une nouvelle fonction compatible avec le nouveau format + amélioration contrôleurs et vues de ModifierMonInscription, CréerMonInscription, ModifierReglementsRemboursements + création d'un nouveau dossier comportant les exports
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Amélioration des contrôleurs et vues Modifier/Supprimer un Eleve/Admin et de la classe DAO + mise à jour de la liste des tâches.
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24450" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>mdp : Sio1_Sio2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Exporter des données</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +943,7 @@
         <v>42516</v>
       </c>
     </row>
-    <row r="33" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -957,7 +960,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="34" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -970,9 +973,9 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -981,39 +984,43 @@
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="9">
+        <v>42522</v>
+      </c>
+      <c r="G35" s="9">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="9">
         <v>42521</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G36" s="9">
         <v>42522</v>
       </c>
     </row>
-    <row r="37" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>12</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>25</v>
@@ -1024,37 +1031,33 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="41" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="42" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>14</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="9">
-        <v>42516</v>
-      </c>
-      <c r="G42" s="9">
-        <v>42516</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>15</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1063,79 +1066,109 @@
         <v>25</v>
       </c>
       <c r="F43" s="9">
-        <v>42517</v>
+        <v>42516</v>
       </c>
       <c r="G43" s="9">
-        <v>42517</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42516</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="46" spans="1:7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="E44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G44" s="9">
+        <v>42517</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="9">
+        <v>42523</v>
+      </c>
+      <c r="G45" s="9">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="9">
-        <v>42517</v>
-      </c>
-      <c r="G47" s="9">
-        <v>42517</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="9">
+        <v>42517</v>
+      </c>
+      <c r="G48" s="9">
+        <v>42517</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-    </row>
+      <c r="E49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="9">
+        <v>42523</v>
+      </c>
+      <c r="G49" s="9">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="9">
+        <v>42523</v>
+      </c>
+      <c r="G50" s="9">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
Améliorations des contrôleurs et vues CreerMonInscription, DemanderCreationCompte, ModifierMonInscription, VoirDetailsSoiree + méthode getSoiree de la classe DAO + Améliorations des "VueMenu"
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24450" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23520" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">      Modifier mon inscription</t>
   </si>
   <si>
-    <t xml:space="preserve">      Annuler mon inscription</t>
-  </si>
-  <si>
     <t>Le réseau des anciens élèves</t>
   </si>
   <si>
@@ -137,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">      Exporter des données</t>
+  </si>
+  <si>
+    <t>Validé HTML</t>
+  </si>
+  <si>
+    <t>Validé JQUERY</t>
   </si>
 </sst>
 </file>
@@ -574,8 +577,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,11 +591,12 @@
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -601,7 +605,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -610,9 +614,9 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -621,7 +625,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
@@ -630,35 +634,41 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -666,7 +676,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="9">
         <v>42512</v>
@@ -674,8 +684,11 @@
       <c r="G9" s="9">
         <v>42512</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -683,7 +696,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="9">
         <v>42512</v>
@@ -691,20 +704,23 @@
       <c r="G10" s="9">
         <v>42512</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="9">
@@ -713,15 +729,16 @@
       <c r="G13" s="9">
         <v>42516</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="9">
@@ -730,16 +747,17 @@
       <c r="G14" s="9">
         <v>42516</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="9">
         <v>42515</v>
@@ -747,15 +765,18 @@
       <c r="G15" s="9">
         <v>42517</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9">
@@ -764,266 +785,273 @@
       <c r="G16" s="9">
         <v>42520</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="9">
-        <v>42517</v>
-      </c>
-      <c r="G17" s="9">
-        <v>42520</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="9">
+        <v>42514</v>
+      </c>
+      <c r="G20" s="9">
+        <v>42514</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="23" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="9">
-        <v>42514</v>
-      </c>
-      <c r="G21" s="9">
-        <v>42514</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    </row>
+    <row r="26" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="9">
+        <v>42512</v>
+      </c>
+      <c r="G27" s="9">
+        <v>42512</v>
+      </c>
     </row>
     <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="9">
-        <v>42512</v>
+        <v>42514</v>
       </c>
       <c r="G28" s="9">
-        <v>42512</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="9">
         <v>42514</v>
       </c>
-      <c r="G29" s="9">
+    </row>
+    <row r="30" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="9">
         <v>42514</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="9">
+        <v>42516</v>
+      </c>
     </row>
     <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F32" s="9">
-        <v>42514</v>
+        <v>42515</v>
       </c>
       <c r="G32" s="9">
-        <v>42516</v>
+        <v>42517</v>
       </c>
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="9">
-        <v>42515</v>
-      </c>
-      <c r="G33" s="9">
-        <v>42517</v>
-      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="9">
+        <v>42522</v>
+      </c>
+      <c r="G34" s="9">
+        <v>42523</v>
+      </c>
     </row>
     <row r="35" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="9">
+        <v>42521</v>
+      </c>
+      <c r="G35" s="9">
         <v>42522</v>
       </c>
-      <c r="G35" s="9">
-        <v>42523</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="9">
-        <v>42521</v>
-      </c>
-      <c r="G36" s="9">
-        <v>42522</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+    </row>
+    <row r="37" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1031,29 +1059,33 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="42" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="9">
+        <v>42516</v>
+      </c>
+      <c r="G42" s="9">
+        <v>42516</v>
+      </c>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1063,13 +1095,13 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F43" s="9">
-        <v>42516</v>
+        <v>42517</v>
       </c>
       <c r="G43" s="9">
-        <v>42516</v>
+        <v>42517</v>
       </c>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1080,42 +1112,42 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44" s="9">
+        <v>42523</v>
+      </c>
+      <c r="G44" s="9">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="9">
         <v>42517</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G47" s="9">
         <v>42517</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="9">
-        <v>42523</v>
-      </c>
-      <c r="G45" s="9">
-        <v>42523</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1125,13 +1157,13 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" s="9">
-        <v>42517</v>
+        <v>42523</v>
       </c>
       <c r="G48" s="9">
-        <v>42517</v>
+        <v>42523</v>
       </c>
     </row>
     <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1174,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F49" s="9">
         <v>42523</v>
@@ -1152,23 +1184,21 @@
       </c>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" s="9">
-        <v>42523</v>
-      </c>
-      <c r="G50" s="9">
-        <v>42523</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
Modification de toutes les vues pour retourner soit au menu soit sur la page en fonction du message (information/avertissement) + modification de la fonction modifierCompteEleve (adrMail) + ajout de l'adrMail dans la modification de la fiche perso d'un elève (contrôleur + vues) + ajout variable titreHeader en jquery pour le header + ajout variable lienRetour dans tous les contrôleurs dont les vues intéragissent avec l'utilisateur + Amélioration de la vue VoirDetailSoiree HTML + maps en jquery (non fonctionnel)
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23520" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,6 +263,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,8 +580,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,15 +598,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -615,15 +618,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -687,26 +690,26 @@
       <c r="H9" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="I9" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="9">
         <v>42512</v>
       </c>
-      <c r="G10" s="9">
-        <v>42512</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -729,7 +732,10 @@
       <c r="G13" s="9">
         <v>42516</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -747,7 +753,10 @@
       <c r="G14" s="9">
         <v>42516</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -768,6 +777,7 @@
       <c r="H15" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -786,6 +796,7 @@
         <v>42520</v>
       </c>
       <c r="H16" s="5"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="18" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -811,6 +822,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -831,6 +843,7 @@
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -845,6 +858,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="23" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -912,6 +926,7 @@
       <c r="G27" s="9">
         <v>42512</v>
       </c>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -929,6 +944,7 @@
       <c r="G28" s="9">
         <v>42514</v>
       </c>
+      <c r="H28" s="5"/>
     </row>
     <row r="30" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -957,6 +973,7 @@
       <c r="G31" s="9">
         <v>42516</v>
       </c>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -974,6 +991,7 @@
       <c r="G32" s="9">
         <v>42517</v>
       </c>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -987,6 +1005,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1004,6 +1023,7 @@
       <c r="G34" s="9">
         <v>42523</v>
       </c>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1021,6 +1041,7 @@
       <c r="G35" s="9">
         <v>42522</v>
       </c>
+      <c r="H35" s="5"/>
     </row>
     <row r="37" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1045,6 +1066,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1058,6 +1080,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="41" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1086,6 +1109,7 @@
       <c r="G42" s="9">
         <v>42516</v>
       </c>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1103,6 +1127,7 @@
       <c r="G43" s="9">
         <v>42517</v>
       </c>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1120,6 +1145,7 @@
       <c r="G44" s="9">
         <v>42523</v>
       </c>
+      <c r="H44" s="5"/>
     </row>
     <row r="46" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1148,6 +1174,7 @@
       <c r="G47" s="9">
         <v>42517</v>
       </c>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1165,6 +1192,7 @@
       <c r="G48" s="9">
         <v>42523</v>
       </c>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1182,6 +1210,7 @@
       <c r="G49" s="9">
         <v>42523</v>
       </c>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>

</xml_diff>

<commit_message>
Modifications des vérifications faites avec Mr Cartron
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23490" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -210,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -233,11 +233,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -271,6 +293,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,17 +734,21 @@
         <v>3</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F10" s="9">
         <v>42512</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="H10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -722,10 +761,10 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F13" s="9">
         <v>42515</v>
       </c>
@@ -735,7 +774,9 @@
       <c r="H13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -743,10 +784,10 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F14" s="9">
         <v>42516</v>
       </c>
@@ -756,7 +797,9 @@
       <c r="H14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -777,7 +820,9 @@
       <c r="H15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -785,18 +830,22 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F16" s="9">
         <v>42517</v>
       </c>
       <c r="G16" s="9">
         <v>42520</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="11"/>
+      <c r="H16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -843,7 +892,9 @@
       <c r="H20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -898,6 +949,12 @@
       <c r="G24" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="26" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -926,7 +983,12 @@
       <c r="G27" s="9">
         <v>42512</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -944,7 +1006,16 @@
       <c r="G28" s="9">
         <v>42514</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -956,6 +1027,8 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -973,7 +1046,12 @@
       <c r="G31" s="9">
         <v>42516</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -991,7 +1069,12 @@
       <c r="G32" s="9">
         <v>42517</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1006,6 +1089,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1024,6 +1108,7 @@
         <v>42523</v>
       </c>
       <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1038,10 +1123,16 @@
       <c r="F35" s="9">
         <v>42521</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="13">
         <v>42522</v>
       </c>
       <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G36" s="15"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1052,7 +1143,9 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1067,6 +1160,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1079,8 +1173,14 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="14"/>
       <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G40" s="15"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1091,7 +1191,9 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1110,6 +1212,7 @@
         <v>42516</v>
       </c>
       <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1128,6 +1231,7 @@
         <v>42517</v>
       </c>
       <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1146,6 +1250,12 @@
         <v>42523</v>
       </c>
       <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
     </row>
     <row r="46" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1156,7 +1266,10 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="17"/>
     </row>
     <row r="47" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1175,6 +1288,7 @@
         <v>42517</v>
       </c>
       <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1193,6 +1307,7 @@
         <v>42523</v>
       </c>
       <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1211,6 +1326,7 @@
         <v>42523</v>
       </c>
       <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>

</xml_diff>

<commit_message>
Liste des tâches + portail
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23490" windowHeight="8880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20850" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Validé JQUERY</t>
+  </si>
+  <si>
+    <t>Rédaction d'un manuel d'utilisation Mail Chimp</t>
   </si>
 </sst>
 </file>
@@ -290,9 +293,6 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -306,6 +306,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,8 +618,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,15 +636,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -653,15 +656,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -1123,14 +1126,14 @@
       <c r="F35" s="9">
         <v>42521</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="12">
         <v>42522</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="15"/>
+      <c r="G36" s="14"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
@@ -1143,7 +1146,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="16"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
@@ -1173,12 +1176,12 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="14"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="15"/>
+      <c r="G40" s="14"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
@@ -1191,7 +1194,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="16"/>
+      <c r="G41" s="15"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
@@ -1253,9 +1256,9 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1266,10 +1269,10 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="17"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1336,13 +1339,22 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+    <row r="51" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="9">
+        <v>42523</v>
+      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Améliorations de la classe DAO et de quelques vues HTML5 et jquery
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20850" windowHeight="8880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17655" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -124,9 +124,6 @@
     <t xml:space="preserve">      Envoyer un courriel</t>
   </si>
   <si>
-    <t>courriel : une personne, tout le monde, les inscrits, les non inscrits, une année de début de BTS</t>
-  </si>
-  <si>
     <t>Adresse mailchimp : delasalle.sio.destinataire@gmail.com</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Rédaction d'un manuel d'utilisation Mail Chimp</t>
+  </si>
+  <si>
+    <t>AJOUTER TITRE H3</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,10 +698,10 @@
         <v>23</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -915,19 +915,16 @@
       <c r="I21" s="11"/>
     </row>
     <row r="23" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
         <v>36</v>
-      </c>
-      <c r="J23" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -953,10 +950,10 @@
         <v>23</v>
       </c>
       <c r="H24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,14 +1093,14 @@
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F34" s="9">
         <v>42522</v>
       </c>
@@ -1119,10 +1116,10 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F35" s="9">
         <v>42521</v>
       </c>
@@ -1235,6 +1232,9 @@
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
+      <c r="J43" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1254,6 +1254,9 @@
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
+      <c r="J44" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G45" s="15"/>
@@ -1311,6 +1314,9 @@
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
+      <c r="J48" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1330,6 +1336,9 @@
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
+      <c r="J49" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
@@ -1341,18 +1350,20 @@
     </row>
     <row r="51" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="5"/>
-      <c r="C51" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F51" s="9">
         <v>42523</v>
       </c>
-      <c r="G51" s="9"/>
+      <c r="G51" s="9">
+        <v>42534</v>
+      </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
     </row>

</xml_diff>

<commit_message>
Petites améliorations de vue Connecter et vue Menu
</commit_message>
<xml_diff>
--- a/documents/Liste des taches.xlsx
+++ b/documents/Liste des taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17655" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>Gestion du menu élève</t>
   </si>
@@ -142,7 +142,7 @@
     <t>Rédaction d'un manuel d'utilisation Mail Chimp</t>
   </si>
   <si>
-    <t>AJOUTER TITRE H3</t>
+    <t>MAILCHIMP</t>
   </si>
 </sst>
 </file>
@@ -213,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -258,11 +258,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -296,9 +333,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,6 +341,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,8 +661,8 @@
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,15 +679,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
@@ -656,15 +699,15 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -745,7 +788,9 @@
       <c r="F10" s="9">
         <v>42512</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="9">
+        <v>42493</v>
+      </c>
       <c r="H10" s="11" t="s">
         <v>24</v>
       </c>
@@ -903,14 +948,18 @@
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="9">
+        <v>42536</v>
+      </c>
+      <c r="G21" s="9">
+        <v>42541</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="11"/>
     </row>
@@ -1080,16 +1129,16 @@
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="B33" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1130,7 +1179,7 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="14"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
@@ -1143,7 +1192,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="14"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
@@ -1166,19 +1215,23 @@
       <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="13"/>
+      <c r="E39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="9">
+        <v>42538</v>
+      </c>
+      <c r="G39" s="12">
+        <v>42541</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="14"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
@@ -1191,7 +1244,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="15"/>
+      <c r="G41" s="14"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
@@ -1232,9 +1285,6 @@
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1254,14 +1304,11 @@
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1272,10 +1319,10 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="16"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1314,9 +1361,6 @@
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
-      <c r="J48" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1336,9 +1380,6 @@
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-      <c r="J49" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
@@ -1368,9 +1409,10 @@
       <c r="I51" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B33:I33"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" r:id="rId1"/>

</xml_diff>